<commit_message>
git ignore added and some change also
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,18 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +356,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -358,7 +390,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -370,7 +402,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>